<commit_message>
Added anatomy to stim results
</commit_message>
<xml_diff>
--- a/stim_results.xlsx
+++ b/stim_results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jsh3653/Documents/Austin/code/SpeechCortex/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{211EDBF6-30BB-8940-968F-0EA3136CB8E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8E822E6-26EC-7941-A5C5-6E24EFFEB571}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-36600" yWindow="5860" windowWidth="27640" windowHeight="16940" xr2:uid="{2CB8FFC4-ECFC-214E-AD02-C760B8673F1E}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="60">
   <si>
     <t>patient</t>
   </si>
@@ -36,12 +36,18 @@
     <t>S06</t>
   </si>
   <si>
+    <t>pSTG</t>
+  </si>
+  <si>
     <t>interruption: paraphasia</t>
   </si>
   <si>
     <t>naming impairment</t>
   </si>
   <si>
+    <t>aSTG</t>
+  </si>
+  <si>
     <t>interruption: "voice sounds far away"</t>
   </si>
   <si>
@@ -57,6 +63,9 @@
     <t>can't hear; "I can’t get it, like something camouflaging what you are saying"</t>
   </si>
   <si>
+    <t>HG</t>
+  </si>
+  <si>
     <t>hears sounds, repeats accurately</t>
   </si>
   <si>
@@ -81,6 +90,9 @@
     <t>S11</t>
   </si>
   <si>
+    <t>PT</t>
+  </si>
+  <si>
     <t>slight delay; otherwise intact</t>
   </si>
   <si>
@@ -190,6 +202,9 @@
   </si>
   <si>
     <t>z</t>
+  </si>
+  <si>
+    <t>anatomy</t>
   </si>
 </sst>
 </file>
@@ -550,1076 +565,1176 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{684C43AB-82B4-6D44-AEE1-D4BF41D6DA00}">
-  <dimension ref="A1:J33"/>
+  <dimension ref="A1:K33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="9.83203125" style="2" customWidth="1"/>
     <col min="2" max="2" width="4.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="33" style="3" customWidth="1"/>
-    <col min="7" max="7" width="36.33203125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="8.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="33" style="3" customWidth="1"/>
+    <col min="8" max="8" width="36.33203125" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>48</v>
+        <v>51</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>59</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>50</v>
+        <v>53</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>1</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>52</v>
+        <v>54</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>55</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+        <v>57</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="1">
         <v>43</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="1">
         <v>6</v>
       </c>
-      <c r="D2" s="1">
-        <v>50</v>
-      </c>
       <c r="E2" s="1">
-        <v>2</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>27</v>
+        <v>50</v>
+      </c>
+      <c r="F2" s="1">
+        <v>2</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="H2">
+        <v>31</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="I2">
         <v>-67.707999999999998</v>
       </c>
-      <c r="I2">
+      <c r="J2">
         <v>-6.673</v>
       </c>
-      <c r="J2">
+      <c r="K2">
         <v>-15.518000000000001</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="1">
         <v>47</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="1">
         <v>6</v>
       </c>
-      <c r="D3" s="1">
-        <v>50</v>
-      </c>
       <c r="E3" s="1">
-        <v>2</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>27</v>
+        <v>50</v>
+      </c>
+      <c r="F3" s="1">
+        <v>2</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="H3">
+        <v>31</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="I3">
         <v>-67.777000000000001</v>
       </c>
-      <c r="I3">
+      <c r="J3">
         <v>-21.446999999999999</v>
       </c>
-      <c r="J3">
+      <c r="K3">
         <v>-8.1649999999999991</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="1">
         <v>75</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="1">
         <v>7</v>
       </c>
-      <c r="D4" s="1">
-        <v>50</v>
-      </c>
       <c r="E4" s="1">
-        <v>2</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>27</v>
+        <v>50</v>
+      </c>
+      <c r="F4" s="1">
+        <v>2</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="H4">
+        <v>31</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I4">
         <v>-67.619</v>
       </c>
-      <c r="I4">
+      <c r="J4">
         <v>-0.56100000000000005</v>
       </c>
-      <c r="J4">
+      <c r="K4">
         <v>-15.12</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B5" s="1">
         <v>7</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" s="1">
         <v>6</v>
       </c>
-      <c r="D5" s="1">
-        <v>50</v>
-      </c>
       <c r="E5" s="1">
-        <v>2</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>27</v>
+        <v>50</v>
+      </c>
+      <c r="F5" s="1">
+        <v>2</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="H5">
+        <v>31</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I5">
         <v>-60.332999999999998</v>
       </c>
-      <c r="I5">
+      <c r="J5">
         <v>5.4379999999999997</v>
       </c>
-      <c r="J5">
+      <c r="K5">
         <v>-17.277999999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B6" s="1">
         <v>39</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="1">
         <v>5</v>
       </c>
-      <c r="D6" s="1">
-        <v>50</v>
-      </c>
       <c r="E6" s="1">
-        <v>2</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>27</v>
+        <v>50</v>
+      </c>
+      <c r="F6" s="1">
+        <v>2</v>
       </c>
       <c r="G6" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="I6">
+        <v>-61.223999999999997</v>
+      </c>
+      <c r="J6">
+        <v>16.204999999999998</v>
+      </c>
+      <c r="K6">
+        <v>-22.582000000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="H6">
-        <v>-61.223999999999997</v>
-      </c>
-      <c r="I6">
-        <v>16.204999999999998</v>
-      </c>
-      <c r="J6">
-        <v>-22.582000000000001</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="34" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
-        <v>6</v>
       </c>
       <c r="B7" s="1">
         <v>167</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C7" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D7" s="1">
         <v>5</v>
       </c>
-      <c r="D7" s="1">
-        <v>50</v>
-      </c>
       <c r="E7" s="1">
-        <v>2</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>28</v>
+        <v>50</v>
+      </c>
+      <c r="F7" s="1">
+        <v>2</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="H7">
+        <v>32</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I7">
         <v>-67.397000000000006</v>
       </c>
-      <c r="I7">
+      <c r="J7">
         <v>-21.963000000000001</v>
       </c>
-      <c r="J7">
+      <c r="K7">
         <v>-6.407</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B8" s="1">
         <v>265</v>
       </c>
-      <c r="C8" s="1">
-        <v>1</v>
+      <c r="C8" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="D8" s="1">
-        <v>50</v>
+        <v>1</v>
       </c>
       <c r="E8" s="1">
-        <v>1</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>29</v>
+        <v>50</v>
+      </c>
+      <c r="F8" s="1">
+        <v>1</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H8">
+        <v>33</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="I8">
         <v>-33.802999999999997</v>
       </c>
-      <c r="I8">
+      <c r="J8">
         <v>-7.2549999999999999</v>
       </c>
-      <c r="J8">
+      <c r="K8">
         <v>-6.3570000000000002</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" ht="51" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B9" s="1">
         <v>266</v>
       </c>
-      <c r="C9" s="1">
-        <v>1</v>
+      <c r="C9" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="D9" s="1">
-        <v>50</v>
+        <v>1</v>
       </c>
       <c r="E9" s="1">
-        <v>1</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>30</v>
+        <v>50</v>
+      </c>
+      <c r="F9" s="1">
+        <v>1</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H9">
+        <v>34</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="I9">
         <v>-38.972999999999999</v>
       </c>
-      <c r="I9">
+      <c r="J9">
         <v>-4.7859999999999996</v>
       </c>
-      <c r="J9">
+      <c r="K9">
         <v>-6.97</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" ht="51" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B10" s="1">
         <v>267</v>
       </c>
-      <c r="C10" s="1">
-        <v>1</v>
+      <c r="C10" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="D10" s="1">
-        <v>50</v>
+        <v>1</v>
       </c>
       <c r="E10" s="1">
-        <v>1</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>31</v>
+        <v>50</v>
+      </c>
+      <c r="F10" s="1">
+        <v>1</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="H10">
+        <v>35</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="I10">
         <v>-42.329000000000001</v>
       </c>
-      <c r="I10">
+      <c r="J10">
         <v>-2.7909999999999999</v>
       </c>
-      <c r="J10">
+      <c r="K10">
         <v>-8.17</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" ht="51" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B11" s="1">
         <v>268</v>
       </c>
-      <c r="C11" s="1">
-        <v>1</v>
+      <c r="C11" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="D11" s="1">
-        <v>50</v>
+        <v>1</v>
       </c>
       <c r="E11" s="1">
-        <v>1</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>32</v>
+        <v>50</v>
+      </c>
+      <c r="F11" s="1">
+        <v>1</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="H11">
+        <v>36</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I11">
         <v>-43.137999999999998</v>
       </c>
-      <c r="I11">
+      <c r="J11">
         <v>0.67</v>
       </c>
-      <c r="J11">
+      <c r="K11">
         <v>-9.6880000000000006</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B12" s="1">
         <v>269</v>
       </c>
-      <c r="C12" s="1">
-        <v>1</v>
+      <c r="C12" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="D12" s="1">
-        <v>50</v>
+        <v>1</v>
       </c>
       <c r="E12" s="1">
-        <v>1</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>33</v>
+        <v>50</v>
+      </c>
+      <c r="F12" s="1">
+        <v>1</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H12">
+        <v>37</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="I12">
         <v>-45.26</v>
       </c>
-      <c r="I12">
+      <c r="J12">
         <v>7.3890000000000002</v>
       </c>
-      <c r="J12">
+      <c r="K12">
         <v>-9.8829999999999991</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B13" s="1">
         <v>3</v>
       </c>
-      <c r="C13" s="1">
+      <c r="C13" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D13" s="1">
         <v>5</v>
       </c>
-      <c r="D13" s="1">
-        <v>50</v>
-      </c>
       <c r="E13" s="1">
-        <v>2</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>27</v>
+        <v>50</v>
+      </c>
+      <c r="F13" s="1">
+        <v>2</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="H13">
+        <v>31</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="I13">
         <v>-66.281999999999996</v>
       </c>
-      <c r="I13">
+      <c r="J13">
         <v>-29.637</v>
       </c>
-      <c r="J13">
+      <c r="K13">
         <v>-5.3579999999999997</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B14" s="1">
         <v>35</v>
       </c>
-      <c r="C14" s="1">
+      <c r="C14" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D14" s="1">
         <v>4</v>
       </c>
-      <c r="D14" s="1">
-        <v>50</v>
-      </c>
       <c r="E14" s="1">
-        <v>2</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>27</v>
+        <v>50</v>
+      </c>
+      <c r="F14" s="1">
+        <v>2</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="H14">
+        <v>31</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I14">
         <v>-65.674000000000007</v>
       </c>
-      <c r="I14">
+      <c r="J14">
         <v>-22.846</v>
       </c>
-      <c r="J14">
+      <c r="K14">
         <v>-4.6479999999999997</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B15" s="1">
         <v>67</v>
       </c>
-      <c r="C15" s="1">
+      <c r="C15" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D15" s="1">
-        <v>50</v>
+        <v>3</v>
       </c>
       <c r="E15" s="1">
-        <v>2</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>27</v>
+        <v>50</v>
+      </c>
+      <c r="F15" s="1">
+        <v>2</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="H15">
+        <v>31</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="I15">
         <v>-67.406000000000006</v>
       </c>
-      <c r="I15">
+      <c r="J15">
         <v>-17.687999999999999</v>
       </c>
-      <c r="J15">
+      <c r="K15">
         <v>-10.552</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B16" s="1">
         <v>99</v>
       </c>
-      <c r="C16" s="1">
+      <c r="C16" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D16" s="1">
         <v>4</v>
       </c>
-      <c r="D16" s="1">
-        <v>50</v>
-      </c>
       <c r="E16" s="1">
-        <v>2</v>
-      </c>
-      <c r="F16" s="3" t="s">
-        <v>27</v>
+        <v>50</v>
+      </c>
+      <c r="F16" s="1">
+        <v>2</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="H16">
+        <v>31</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I16">
         <v>-67.744</v>
       </c>
-      <c r="I16">
+      <c r="J16">
         <v>-7.9269999999999996</v>
       </c>
-      <c r="J16">
+      <c r="K16">
         <v>-9.4870000000000001</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B17" s="1">
         <v>33</v>
       </c>
-      <c r="C17" s="1">
-        <v>1</v>
+      <c r="C17" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="D17" s="1">
-        <v>50</v>
+        <v>1</v>
       </c>
       <c r="E17" s="1">
-        <v>1</v>
-      </c>
-      <c r="F17" s="3" t="s">
-        <v>34</v>
+        <v>50</v>
+      </c>
+      <c r="F17" s="1">
+        <v>1</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="H17">
+        <v>38</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="I17">
         <v>-49.052</v>
       </c>
-      <c r="I17">
+      <c r="J17">
         <v>7.3390000000000004</v>
       </c>
-      <c r="J17">
+      <c r="K17">
         <v>-20.530999999999999</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B18" s="1">
         <v>34</v>
       </c>
-      <c r="C18" s="1">
-        <v>1</v>
+      <c r="C18" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="D18" s="1">
-        <v>50</v>
+        <v>1</v>
       </c>
       <c r="E18" s="1">
-        <v>1</v>
-      </c>
-      <c r="F18" s="3" t="s">
-        <v>35</v>
+        <v>50</v>
+      </c>
+      <c r="F18" s="1">
+        <v>1</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="H18">
+        <v>39</v>
+      </c>
+      <c r="H18" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="I18">
         <v>-45.545999999999999</v>
       </c>
-      <c r="I18">
+      <c r="J18">
         <v>11.573</v>
       </c>
-      <c r="J18">
+      <c r="K18">
         <v>-20.843</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B19" s="1">
         <v>66</v>
       </c>
-      <c r="C19" s="1">
-        <v>1</v>
+      <c r="C19" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="D19" s="1">
-        <v>50</v>
+        <v>1</v>
       </c>
       <c r="E19" s="1">
-        <v>1</v>
-      </c>
-      <c r="F19" s="3" t="s">
-        <v>36</v>
+        <v>50</v>
+      </c>
+      <c r="F19" s="1">
+        <v>1</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="H19">
+        <v>40</v>
+      </c>
+      <c r="H19" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="I19">
         <v>-42.683</v>
       </c>
-      <c r="I19">
+      <c r="J19">
         <v>-9.9979999999999993</v>
       </c>
-      <c r="J19">
+      <c r="K19">
         <v>-23.120999999999999</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B20" s="1">
         <v>67</v>
       </c>
-      <c r="C20" s="1">
-        <v>1</v>
+      <c r="C20" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="D20" s="1">
-        <v>50</v>
+        <v>1</v>
       </c>
       <c r="E20" s="1">
+        <v>50</v>
+      </c>
+      <c r="F20" s="1">
         <v>3</v>
       </c>
-      <c r="F20" s="3" t="s">
-        <v>37</v>
-      </c>
       <c r="G20" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="H20">
+        <v>41</v>
+      </c>
+      <c r="H20" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="I20">
         <v>-44.061</v>
       </c>
-      <c r="I20">
+      <c r="J20">
         <v>-6.5880000000000001</v>
       </c>
-      <c r="J20">
+      <c r="K20">
         <v>-23.225000000000001</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B21" s="1">
         <v>68</v>
       </c>
-      <c r="C21" s="1">
-        <v>1</v>
+      <c r="C21" s="2" t="s">
+        <v>21</v>
       </c>
       <c r="D21" s="1">
-        <v>50</v>
+        <v>1</v>
       </c>
       <c r="E21" s="1">
+        <v>50</v>
+      </c>
+      <c r="F21" s="1">
         <v>3</v>
       </c>
-      <c r="F21" s="3" t="s">
-        <v>38</v>
-      </c>
       <c r="G21" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="H21">
+        <v>42</v>
+      </c>
+      <c r="H21" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I21">
         <v>-46.408999999999999</v>
       </c>
-      <c r="I21">
+      <c r="J21">
         <v>-3.8180000000000001</v>
       </c>
-      <c r="J21">
+      <c r="K21">
         <v>-21.925000000000001</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B22" s="1">
         <v>69</v>
       </c>
-      <c r="C22" s="1">
-        <v>1</v>
+      <c r="C22" s="2" t="s">
+        <v>21</v>
       </c>
       <c r="D22" s="1">
-        <v>50</v>
+        <v>1</v>
       </c>
       <c r="E22" s="1">
+        <v>50</v>
+      </c>
+      <c r="F22" s="1">
         <v>3</v>
       </c>
-      <c r="F22" s="3" t="s">
-        <v>39</v>
-      </c>
       <c r="G22" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="H22">
+        <v>43</v>
+      </c>
+      <c r="H22" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I22">
         <v>-48.866999999999997</v>
       </c>
-      <c r="I22">
+      <c r="J22">
         <v>-5.5E-2</v>
       </c>
-      <c r="J22">
+      <c r="K22">
         <v>-22.507000000000001</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B23" s="1">
         <v>71</v>
       </c>
-      <c r="C23" s="1">
-        <v>2</v>
+      <c r="C23" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="D23" s="1">
-        <v>50</v>
+        <v>2</v>
       </c>
       <c r="E23" s="1">
-        <v>2</v>
-      </c>
-      <c r="F23" s="3" t="s">
-        <v>27</v>
+        <v>50</v>
+      </c>
+      <c r="F23" s="1">
+        <v>2</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="H23">
+        <v>31</v>
+      </c>
+      <c r="H23" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="I23">
         <v>-52.871000000000002</v>
       </c>
-      <c r="I23">
+      <c r="J23">
         <v>7.5960000000000001</v>
       </c>
-      <c r="J23">
+      <c r="K23">
         <v>-22.725000000000001</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B24" s="1">
         <v>72</v>
       </c>
-      <c r="C24" s="1">
-        <v>2</v>
+      <c r="C24" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="D24" s="1">
-        <v>50</v>
+        <v>2</v>
       </c>
       <c r="E24" s="1">
-        <v>2</v>
-      </c>
-      <c r="F24" s="3" t="s">
-        <v>27</v>
+        <v>50</v>
+      </c>
+      <c r="F24" s="1">
+        <v>2</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="H24">
+        <v>31</v>
+      </c>
+      <c r="H24" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="I24">
         <v>-55.305999999999997</v>
       </c>
-      <c r="I24">
+      <c r="J24">
         <v>9.2089999999999996</v>
       </c>
-      <c r="J24">
+      <c r="K24">
         <v>-22.015999999999998</v>
       </c>
     </row>
-    <row r="25" spans="1:10" ht="68" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:11" ht="68" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="B25" s="1">
         <v>105</v>
       </c>
-      <c r="C25" s="1">
+      <c r="C25" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D25" s="1">
-        <v>50</v>
+        <v>3</v>
       </c>
       <c r="E25" s="1">
-        <v>2</v>
-      </c>
-      <c r="F25" s="3" t="s">
-        <v>27</v>
+        <v>50</v>
+      </c>
+      <c r="F25" s="1">
+        <v>2</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="H25">
+        <v>31</v>
+      </c>
+      <c r="H25" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="I25">
         <v>-67.578999999999994</v>
       </c>
-      <c r="I25">
+      <c r="J25">
         <v>-20.66</v>
       </c>
-      <c r="J25">
+      <c r="K25">
         <v>-5.7560000000000002</v>
       </c>
     </row>
-    <row r="26" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="B26" s="1">
         <v>431</v>
       </c>
-      <c r="C26" s="1">
-        <v>1</v>
+      <c r="C26" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="D26" s="1">
-        <v>50</v>
+        <v>1</v>
       </c>
       <c r="E26" s="1">
-        <v>1</v>
-      </c>
-      <c r="F26" s="3" t="s">
-        <v>23</v>
+        <v>50</v>
+      </c>
+      <c r="F26" s="1">
+        <v>1</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="H26">
+        <v>27</v>
+      </c>
+      <c r="H26" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I26">
         <v>-31.792999999999999</v>
       </c>
-      <c r="I26">
+      <c r="J26">
         <v>2.157</v>
       </c>
-      <c r="J26">
+      <c r="K26">
         <v>-17.556999999999999</v>
       </c>
     </row>
-    <row r="27" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="B27" s="1">
         <v>433</v>
       </c>
-      <c r="C27" s="1">
-        <v>1</v>
+      <c r="C27" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="D27" s="1">
-        <v>50</v>
+        <v>1</v>
       </c>
       <c r="E27" s="1">
-        <v>1</v>
-      </c>
-      <c r="F27" s="3" t="s">
-        <v>40</v>
+        <v>50</v>
+      </c>
+      <c r="F27" s="1">
+        <v>1</v>
       </c>
       <c r="G27" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="H27" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="I27">
+        <v>-46.78</v>
+      </c>
+      <c r="J27">
+        <v>4.9820000000000002</v>
+      </c>
+      <c r="K27">
+        <v>-9.4309999999999992</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="A28" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="H27">
-        <v>-46.78</v>
-      </c>
-      <c r="I27">
-        <v>4.9820000000000002</v>
-      </c>
-      <c r="J27">
-        <v>-9.4309999999999992</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A28" s="1" t="s">
-        <v>21</v>
       </c>
       <c r="B28" s="1">
         <v>435</v>
       </c>
-      <c r="C28" s="1">
-        <v>2</v>
+      <c r="C28" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="D28" s="1">
-        <v>50</v>
+        <v>2</v>
       </c>
       <c r="E28" s="1">
-        <v>1</v>
-      </c>
-      <c r="F28" s="3" t="s">
-        <v>41</v>
+        <v>50</v>
+      </c>
+      <c r="F28" s="1">
+        <v>1</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="H28">
+        <v>45</v>
+      </c>
+      <c r="H28" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="I28">
         <v>-54.436999999999998</v>
       </c>
-      <c r="I28">
+      <c r="J28">
         <v>0.96499999999999997</v>
       </c>
-      <c r="J28">
+      <c r="K28">
         <v>-6.665</v>
       </c>
     </row>
-    <row r="29" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B29" s="1">
         <v>12</v>
       </c>
-      <c r="C29" s="1">
+      <c r="C29" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D29" s="1">
         <v>3</v>
       </c>
-      <c r="D29" s="1">
-        <v>50</v>
-      </c>
       <c r="E29" s="1">
-        <v>1</v>
-      </c>
-      <c r="F29" s="3" t="s">
-        <v>42</v>
+        <v>50</v>
+      </c>
+      <c r="F29" s="1">
+        <v>1</v>
       </c>
       <c r="G29" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="H29">
+      <c r="H29" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="I29">
         <v>-39.399000000000001</v>
       </c>
-      <c r="I29">
+      <c r="J29">
         <v>-4.3949999999999996</v>
       </c>
-      <c r="J29">
+      <c r="K29">
         <v>-9.1319999999999997</v>
       </c>
     </row>
-    <row r="30" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B30" s="1">
         <v>13</v>
       </c>
-      <c r="C30" s="1">
-        <v>2</v>
+      <c r="C30" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="D30" s="1">
-        <v>50</v>
+        <v>2</v>
       </c>
       <c r="E30" s="1">
-        <v>1</v>
-      </c>
-      <c r="F30" s="3" t="s">
-        <v>42</v>
+        <v>50</v>
+      </c>
+      <c r="F30" s="1">
+        <v>1</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="H30">
+        <v>46</v>
+      </c>
+      <c r="H30" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="I30">
         <v>-43.140999999999998</v>
       </c>
-      <c r="I30">
+      <c r="J30">
         <v>-9.2949999999999999</v>
       </c>
-      <c r="J30">
+      <c r="K30">
         <v>-13.221</v>
       </c>
     </row>
-    <row r="31" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B31" s="1">
         <v>14</v>
       </c>
-      <c r="C31" s="1">
+      <c r="C31" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D31" s="1">
         <v>3</v>
       </c>
-      <c r="D31" s="1">
-        <v>50</v>
-      </c>
       <c r="E31" s="1">
-        <v>1</v>
-      </c>
-      <c r="F31" s="3" t="s">
-        <v>42</v>
+        <v>50</v>
+      </c>
+      <c r="F31" s="1">
+        <v>1</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="H31">
+        <v>46</v>
+      </c>
+      <c r="H31" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="I31">
         <v>-47.853000000000002</v>
       </c>
-      <c r="I31">
+      <c r="J31">
         <v>-1.55</v>
       </c>
-      <c r="J31">
+      <c r="K31">
         <v>-12.241</v>
       </c>
     </row>
-    <row r="32" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B32" s="1">
         <v>23</v>
       </c>
-      <c r="C32" s="1">
+      <c r="C32" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D32" s="1">
         <v>4</v>
       </c>
-      <c r="D32" s="1">
-        <v>50</v>
-      </c>
       <c r="E32" s="1">
-        <v>1</v>
-      </c>
-      <c r="F32" s="3" t="s">
-        <v>43</v>
+        <v>50</v>
+      </c>
+      <c r="F32" s="1">
+        <v>1</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="H32">
+        <v>47</v>
+      </c>
+      <c r="H32" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="I32">
         <v>-41.963999999999999</v>
       </c>
-      <c r="I32">
+      <c r="J32">
         <v>-8.2439999999999998</v>
       </c>
-      <c r="J32">
+      <c r="K32">
         <v>-4.6980000000000004</v>
       </c>
     </row>
-    <row r="33" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B33" s="1">
         <v>24</v>
       </c>
-      <c r="C33" s="1">
+      <c r="C33" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D33" s="1">
         <v>4</v>
       </c>
-      <c r="D33" s="1">
-        <v>50</v>
-      </c>
       <c r="E33" s="1">
-        <v>1</v>
-      </c>
-      <c r="F33" s="3" t="s">
-        <v>44</v>
+        <v>50</v>
+      </c>
+      <c r="F33" s="1">
+        <v>1</v>
       </c>
       <c r="G33" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="H33">
+        <v>48</v>
+      </c>
+      <c r="H33" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="I33">
         <v>-45.698999999999998</v>
       </c>
-      <c r="I33">
+      <c r="J33">
         <v>-10.124000000000001</v>
       </c>
-      <c r="J33">
+      <c r="K33">
         <v>2.3820000000000001</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Projected electrodes outside of the middle of the mesh
</commit_message>
<xml_diff>
--- a/stim_results.xlsx
+++ b/stim_results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jsh3653/Documents/Austin/code/SpeechCortex/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54745B55-5426-1142-B714-D053796786AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F2CFF2F-B2AA-8749-B053-9A8AC29717E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-36600" yWindow="5860" windowWidth="27640" windowHeight="16940" xr2:uid="{2CB8FFC4-ECFC-214E-AD02-C760B8673F1E}"/>
   </bookViews>
@@ -568,7 +568,7 @@
   <dimension ref="A1:K33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2:K33"/>
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -644,13 +644,13 @@
         <v>4</v>
       </c>
       <c r="I2">
-        <v>-67.708200000000005</v>
+        <v>-68.395700000000005</v>
       </c>
       <c r="J2">
-        <v>-6.6731999999999996</v>
+        <v>-8.5576000000000008</v>
       </c>
       <c r="K2">
-        <v>-15.5175</v>
+        <v>-13.580299999999999</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="17" x14ac:dyDescent="0.2">
@@ -679,13 +679,13 @@
         <v>5</v>
       </c>
       <c r="I3">
-        <v>-67.777299999999997</v>
+        <v>-67.773200000000003</v>
       </c>
       <c r="J3">
-        <v>-21.4467</v>
+        <v>-22.257400000000001</v>
       </c>
       <c r="K3">
-        <v>-8.1646999999999998</v>
+        <v>-7.6257000000000001</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="17" x14ac:dyDescent="0.2">
@@ -749,13 +749,13 @@
         <v>9</v>
       </c>
       <c r="I5">
-        <v>-60.332799999999999</v>
+        <v>-66.544899999999998</v>
       </c>
       <c r="J5">
-        <v>5.4382000000000001</v>
+        <v>2.7523</v>
       </c>
       <c r="K5">
-        <v>-17.277699999999999</v>
+        <v>-15.3057</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="34" x14ac:dyDescent="0.2">
@@ -784,13 +784,13 @@
         <v>10</v>
       </c>
       <c r="I6">
-        <v>-61.223599999999998</v>
+        <v>-61.795699999999997</v>
       </c>
       <c r="J6">
-        <v>16.204899999999999</v>
+        <v>15.499599999999999</v>
       </c>
       <c r="K6">
-        <v>-22.582000000000001</v>
+        <v>-20.139800000000001</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="34" x14ac:dyDescent="0.2">
@@ -819,13 +819,13 @@
         <v>11</v>
       </c>
       <c r="I7">
-        <v>-67.396600000000007</v>
+        <v>-67.751099999999994</v>
       </c>
       <c r="J7">
-        <v>-21.962900000000001</v>
+        <v>-21.2439</v>
       </c>
       <c r="K7">
-        <v>-6.4066000000000001</v>
+        <v>-7.0552000000000001</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="34" x14ac:dyDescent="0.2">
@@ -854,13 +854,13 @@
         <v>13</v>
       </c>
       <c r="I8">
-        <v>-35.040999999999997</v>
+        <v>-31.254000000000001</v>
       </c>
       <c r="J8">
-        <v>-8.2565000000000008</v>
+        <v>-11.762700000000001</v>
       </c>
       <c r="K8">
-        <v>-6.6520999999999999</v>
+        <v>-4.7976999999999999</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="51" x14ac:dyDescent="0.2">
@@ -889,13 +889,13 @@
         <v>13</v>
       </c>
       <c r="I9">
-        <v>-39.213999999999999</v>
+        <v>-31.254000000000001</v>
       </c>
       <c r="J9">
-        <v>-5.4550999999999998</v>
+        <v>-11.762700000000001</v>
       </c>
       <c r="K9">
-        <v>-8.0390999999999995</v>
+        <v>-4.7976999999999999</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="51" x14ac:dyDescent="0.2">
@@ -924,13 +924,13 @@
         <v>14</v>
       </c>
       <c r="I10">
-        <v>-42.7181</v>
+        <v>-31.254000000000001</v>
       </c>
       <c r="J10">
-        <v>-3.0293999999999999</v>
+        <v>-11.762700000000001</v>
       </c>
       <c r="K10">
-        <v>-8.3173999999999992</v>
+        <v>-4.7976999999999999</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="51" x14ac:dyDescent="0.2">
@@ -959,13 +959,13 @@
         <v>15</v>
       </c>
       <c r="I11">
-        <v>-43.981099999999998</v>
+        <v>-31.254000000000001</v>
       </c>
       <c r="J11">
-        <v>-0.40239999999999998</v>
+        <v>-11.762700000000001</v>
       </c>
       <c r="K11">
-        <v>-10.0304</v>
+        <v>-4.7976999999999999</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="34" x14ac:dyDescent="0.2">
@@ -994,13 +994,13 @@
         <v>16</v>
       </c>
       <c r="I12">
-        <v>-47.979599999999998</v>
+        <v>-58.363599999999998</v>
       </c>
       <c r="J12">
-        <v>4.6821999999999999</v>
+        <v>16.240300000000001</v>
       </c>
       <c r="K12">
-        <v>-12.7293</v>
+        <v>-17.109100000000002</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="17" x14ac:dyDescent="0.2">
@@ -1029,13 +1029,13 @@
         <v>49</v>
       </c>
       <c r="I13">
-        <v>-66.282300000000006</v>
+        <v>-66.228700000000003</v>
       </c>
       <c r="J13">
-        <v>-29.636600000000001</v>
+        <v>-30.240100000000002</v>
       </c>
       <c r="K13">
-        <v>-5.3582999999999998</v>
+        <v>-3.3279999999999998</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="17" x14ac:dyDescent="0.2">
@@ -1064,13 +1064,13 @@
         <v>18</v>
       </c>
       <c r="I14">
-        <v>-65.673900000000003</v>
+        <v>-67.751099999999994</v>
       </c>
       <c r="J14">
-        <v>-22.846</v>
+        <v>-21.2439</v>
       </c>
       <c r="K14">
-        <v>-4.6483999999999996</v>
+        <v>-7.0552000000000001</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="17" x14ac:dyDescent="0.2">
@@ -1099,13 +1099,13 @@
         <v>19</v>
       </c>
       <c r="I15">
-        <v>-67.406300000000002</v>
+        <v>-67.751099999999994</v>
       </c>
       <c r="J15">
-        <v>-17.687799999999999</v>
+        <v>-21.2439</v>
       </c>
       <c r="K15">
-        <v>-10.552199999999999</v>
+        <v>-7.0552000000000001</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="17" x14ac:dyDescent="0.2">
@@ -1134,13 +1134,13 @@
         <v>18</v>
       </c>
       <c r="I16">
-        <v>-67.743600000000001</v>
+        <v>-67.860500000000002</v>
       </c>
       <c r="J16">
-        <v>-7.9272</v>
+        <v>-6.8452000000000002</v>
       </c>
       <c r="K16">
-        <v>-9.4867000000000008</v>
+        <v>-10.079499999999999</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="17" x14ac:dyDescent="0.2">
@@ -1169,13 +1169,13 @@
         <v>32</v>
       </c>
       <c r="I17">
-        <v>-46.039200000000001</v>
+        <v>-58.363599999999998</v>
       </c>
       <c r="J17">
-        <v>7.2098000000000004</v>
+        <v>16.240300000000001</v>
       </c>
       <c r="K17">
-        <v>-19.691600000000001</v>
+        <v>-17.109100000000002</v>
       </c>
     </row>
     <row r="18" spans="1:11" ht="17" x14ac:dyDescent="0.2">
@@ -1204,13 +1204,13 @@
         <v>32</v>
       </c>
       <c r="I18">
-        <v>-46.911799999999999</v>
+        <v>-58.363599999999998</v>
       </c>
       <c r="J18">
-        <v>12.6113</v>
+        <v>16.240300000000001</v>
       </c>
       <c r="K18">
-        <v>-21.638999999999999</v>
+        <v>-17.109100000000002</v>
       </c>
     </row>
     <row r="19" spans="1:11" ht="17" x14ac:dyDescent="0.2">
@@ -1239,13 +1239,13 @@
         <v>32</v>
       </c>
       <c r="I19">
-        <v>-45.018300000000004</v>
+        <v>-31.9497</v>
       </c>
       <c r="J19">
-        <v>-10.6807</v>
+        <v>-12.861599999999999</v>
       </c>
       <c r="K19">
-        <v>-23.408899999999999</v>
+        <v>-2.8336999999999999</v>
       </c>
     </row>
     <row r="20" spans="1:11" ht="17" x14ac:dyDescent="0.2">
@@ -1274,13 +1274,13 @@
         <v>32</v>
       </c>
       <c r="I20">
-        <v>-46.500700000000002</v>
+        <v>-31.254000000000001</v>
       </c>
       <c r="J20">
-        <v>-8.8794000000000004</v>
+        <v>-11.762700000000001</v>
       </c>
       <c r="K20">
-        <v>-23.429500000000001</v>
+        <v>-4.7976999999999999</v>
       </c>
     </row>
     <row r="21" spans="1:11" ht="17" x14ac:dyDescent="0.2">
@@ -1309,13 +1309,13 @@
         <v>22</v>
       </c>
       <c r="I21">
-        <v>-48.327599999999997</v>
+        <v>-63.590200000000003</v>
       </c>
       <c r="J21">
-        <v>-5.3033000000000001</v>
+        <v>-2.6019999999999999</v>
       </c>
       <c r="K21">
-        <v>-23.895099999999999</v>
+        <v>-7.5965999999999996</v>
       </c>
     </row>
     <row r="22" spans="1:11" ht="17" x14ac:dyDescent="0.2">
@@ -1344,13 +1344,13 @@
         <v>22</v>
       </c>
       <c r="I22">
-        <v>-49.802999999999997</v>
+        <v>-63.590200000000003</v>
       </c>
       <c r="J22">
-        <v>1.7639</v>
+        <v>-2.6019999999999999</v>
       </c>
       <c r="K22">
-        <v>-24.732500000000002</v>
+        <v>-7.5965999999999996</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="34" x14ac:dyDescent="0.2">
@@ -1379,13 +1379,13 @@
         <v>23</v>
       </c>
       <c r="I23">
-        <v>-53.305599999999998</v>
+        <v>-58.363599999999998</v>
       </c>
       <c r="J23">
-        <v>6.2008999999999999</v>
+        <v>16.240300000000001</v>
       </c>
       <c r="K23">
-        <v>-24.7774</v>
+        <v>-17.109100000000002</v>
       </c>
     </row>
     <row r="24" spans="1:11" ht="34" x14ac:dyDescent="0.2">
@@ -1414,13 +1414,13 @@
         <v>24</v>
       </c>
       <c r="I24">
-        <v>-56.769399999999997</v>
+        <v>-58.363599999999998</v>
       </c>
       <c r="J24">
-        <v>7.5559000000000003</v>
+        <v>16.240300000000001</v>
       </c>
       <c r="K24">
-        <v>-24.565000000000001</v>
+        <v>-17.109100000000002</v>
       </c>
     </row>
     <row r="25" spans="1:11" ht="68" x14ac:dyDescent="0.2">
@@ -1449,13 +1449,13 @@
         <v>26</v>
       </c>
       <c r="I25">
-        <v>-67.579499999999996</v>
+        <v>-67.751099999999994</v>
       </c>
       <c r="J25">
-        <v>-20.659800000000001</v>
+        <v>-21.2439</v>
       </c>
       <c r="K25">
-        <v>-5.7561999999999998</v>
+        <v>-7.0552000000000001</v>
       </c>
     </row>
     <row r="26" spans="1:11" ht="17" x14ac:dyDescent="0.2">
@@ -1484,13 +1484,13 @@
         <v>28</v>
       </c>
       <c r="I26">
-        <v>-40.019300000000001</v>
+        <v>-31.254000000000001</v>
       </c>
       <c r="J26">
-        <v>-2.5017</v>
+        <v>-11.762700000000001</v>
       </c>
       <c r="K26">
-        <v>-16.806000000000001</v>
+        <v>-4.7976999999999999</v>
       </c>
     </row>
     <row r="27" spans="1:11" ht="17" x14ac:dyDescent="0.2">
@@ -1519,13 +1519,13 @@
         <v>29</v>
       </c>
       <c r="I27">
-        <v>-48.217500000000001</v>
+        <v>-58.363599999999998</v>
       </c>
       <c r="J27">
-        <v>3.1198000000000001</v>
+        <v>16.240300000000001</v>
       </c>
       <c r="K27">
-        <v>-11.4459</v>
+        <v>-17.109100000000002</v>
       </c>
     </row>
     <row r="28" spans="1:11" ht="17" x14ac:dyDescent="0.2">
@@ -1554,13 +1554,13 @@
         <v>29</v>
       </c>
       <c r="I28">
-        <v>-55.354100000000003</v>
+        <v>-63.590200000000003</v>
       </c>
       <c r="J28">
-        <v>-1.2781</v>
+        <v>-2.6019999999999999</v>
       </c>
       <c r="K28">
-        <v>-9.8916000000000004</v>
+        <v>-7.5965999999999996</v>
       </c>
     </row>
     <row r="29" spans="1:11" ht="34" x14ac:dyDescent="0.2">
@@ -1589,13 +1589,13 @@
         <v>50</v>
       </c>
       <c r="I29">
-        <v>-39.597900000000003</v>
+        <v>-31.254000000000001</v>
       </c>
       <c r="J29">
-        <v>-4.4090999999999996</v>
+        <v>-11.762700000000001</v>
       </c>
       <c r="K29">
-        <v>-9.4928000000000008</v>
+        <v>-4.7976999999999999</v>
       </c>
     </row>
     <row r="30" spans="1:11" ht="17" x14ac:dyDescent="0.2">
@@ -1624,13 +1624,13 @@
         <v>29</v>
       </c>
       <c r="I30">
-        <v>-46.004899999999999</v>
+        <v>-31.9497</v>
       </c>
       <c r="J30">
-        <v>-9.9682999999999993</v>
+        <v>-12.861599999999999</v>
       </c>
       <c r="K30">
-        <v>-11.240600000000001</v>
+        <v>-2.8336999999999999</v>
       </c>
     </row>
     <row r="31" spans="1:11" ht="17" x14ac:dyDescent="0.2">
@@ -1659,13 +1659,13 @@
         <v>29</v>
       </c>
       <c r="I31">
-        <v>-48.8416</v>
+        <v>-63.590200000000003</v>
       </c>
       <c r="J31">
-        <v>-2.3277999999999999</v>
+        <v>-2.6019999999999999</v>
       </c>
       <c r="K31">
-        <v>-10.9551</v>
+        <v>-7.5965999999999996</v>
       </c>
     </row>
     <row r="32" spans="1:11" ht="34" x14ac:dyDescent="0.2">
@@ -1694,13 +1694,13 @@
         <v>29</v>
       </c>
       <c r="I32">
-        <v>-41.8292</v>
+        <v>-31.9497</v>
       </c>
       <c r="J32">
-        <v>-8.2670999999999992</v>
+        <v>-12.861599999999999</v>
       </c>
       <c r="K32">
-        <v>-5.7850999999999999</v>
+        <v>-2.8336999999999999</v>
       </c>
     </row>
     <row r="33" spans="1:11" ht="34" x14ac:dyDescent="0.2">
@@ -1729,13 +1729,13 @@
         <v>29</v>
       </c>
       <c r="I33">
-        <v>-41.743200000000002</v>
+        <v>-32.891800000000003</v>
       </c>
       <c r="J33">
-        <v>-9.7029999999999994</v>
+        <v>-14.9907</v>
       </c>
       <c r="K33">
-        <v>-5.6454000000000004</v>
+        <v>-1.5783</v>
       </c>
     </row>
   </sheetData>

</xml_diff>